<commit_message>
commit to update the way DOC its being save in the df. Now all PDFs and DOCs are saved as string
</commit_message>
<xml_diff>
--- a/Project Report/NLP project Schedule.xlsx
+++ b/Project Report/NLP project Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renzocastagnino/Google Drive/MASTER DATA SCIENCE/SEMESTER 2/Natural Language Process/Project/Project Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D86F94-AD95-6B40-9C68-E4609A5C4CDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C73A948-7028-9B4C-BEFD-BDDC9A5F95CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Presentation</t>
   </si>
@@ -136,6 +136,18 @@
   </si>
   <si>
     <t>Final report - Code and Analysis</t>
+  </si>
+  <si>
+    <t>On track</t>
+  </si>
+  <si>
+    <t>Delayed</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Color Meaning</t>
   </si>
 </sst>
 </file>
@@ -181,7 +193,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,13 +214,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -240,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -264,10 +288,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -280,7 +300,24 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,188 +598,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:N29"/>
+  <dimension ref="B3:O33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="136" workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="29.83203125" customWidth="1"/>
-    <col min="5" max="14" width="10.6640625" customWidth="1"/>
-    <col min="15" max="15" width="22.83203125" customWidth="1"/>
+    <col min="5" max="15" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14" ht="91" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="13" t="s">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C3" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C4" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="20"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C6" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="8" spans="2:15" ht="91" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="N8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="13" t="s">
+      <c r="O8" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B5" s="16" t="s">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E9" s="12">
         <v>43745</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F9" s="12">
         <v>43749</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G9" s="12">
         <v>43752</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H9" s="12">
         <v>43756</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I9" s="12">
         <v>43759</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J9" s="12">
         <v>43770</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K9" s="12">
         <v>43773</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L9" s="12">
+        <v>43780</v>
+      </c>
+      <c r="M9" s="12">
         <v>43787</v>
       </c>
-      <c r="M5" s="14">
+      <c r="N9" s="12">
         <v>43801</v>
       </c>
-      <c r="N5" s="14">
+      <c r="O9" s="12">
         <v>43808</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B6" s="4"/>
-      <c r="C6" s="9" t="s">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="C10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-    </row>
-    <row r="8" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="4">
-        <v>2</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B9" s="4">
-        <v>3</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B10" s="4">
-        <v>4</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -751,139 +736,146 @@
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O10" s="7"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O11" s="7"/>
+    </row>
+    <row r="12" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="6"/>
+      <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O13" s="7"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="6"/>
+      <c r="L14" s="7"/>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O14" s="7"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15" s="4">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
-      <c r="M15" s="6"/>
+      <c r="M15" s="7"/>
       <c r="N15" s="7"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O15" s="7"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16" s="4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
       <c r="M16" s="7"/>
-      <c r="N16" s="6"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" s="4">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>21</v>
@@ -894,17 +886,18 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O17" s="7"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" s="4">
-        <v>12</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>21</v>
@@ -917,20 +910,21 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
+      <c r="M18" s="6"/>
       <c r="N18" s="7"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O18" s="7"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="4">
-        <v>12</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="11"/>
+        <v>21</v>
+      </c>
+      <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -939,161 +933,169 @@
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="N19" s="6"/>
+      <c r="O19" s="7"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="4">
-        <v>12</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O20" s="6"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" s="4">
-        <v>12</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>28</v>
+        <v>11</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O21" s="7"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="4">
         <v>12</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>29</v>
+      <c r="C22" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O22" s="7"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="4">
         <v>12</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="E23" s="17"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O23" s="7"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" s="4">
         <v>12</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O24" s="7"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="4">
         <v>12</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
       <c r="N25" s="7"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O25" s="7"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B26" s="4">
         <v>12</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B27" s="4">
         <v>12</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>21</v>
@@ -1102,46 +1104,137 @@
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
+      <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B28" s="4">
         <v>12</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="4"/>
+      <c r="C28" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O28" s="7"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B29" s="4">
         <v>12</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="4"/>
+      <c r="C29" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B30" s="4">
+        <v>12</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B31" s="4">
+        <v>12</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B32" s="4">
+        <v>12</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B33" s="4">
+        <v>12</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>